<commit_message>
Add test on Viterbi
</commit_message>
<xml_diff>
--- a/src/test/resources/jacobi/test/data/ViterbiTest.xlsx
+++ b/src/test/resources/jacobi/test/data/ViterbiTest.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deveykchan1\git\jacobi\src\test\resources\jacobi\test\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="test DNA GC Content #1" sheetId="1" r:id="rId1"/>
+    <sheet name="Muller, FMP, Springer 2015" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t xml:space="preserve">Initial </t>
   </si>
@@ -96,6 +92,66 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>A1A2A3</t>
+  </si>
+  <si>
+    <t>B1B2B3</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Encode</t>
+  </si>
+  <si>
+    <t>Emit By</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>Backtrack</t>
+  </si>
+  <si>
+    <t>Hidden sequence</t>
+  </si>
+  <si>
+    <t>#100</t>
+  </si>
+  <si>
+    <t>Encoded</t>
+  </si>
+  <si>
+    <t>DP Table</t>
   </si>
 </sst>
 </file>
@@ -149,6 +205,110 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>60333</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>586021</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38098</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11033133" y="171449"/>
+          <a:ext cx="6621688" cy="3105149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>29436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>71780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11058524" y="3429861"/>
+          <a:ext cx="6600825" cy="2147369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -192,7 +352,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,7 +387,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -412,11 +572,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -938,7 +1096,7 @@
         <v>-3.7942399697717626</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:P25" ca="1" si="10">MAX(I25+$I8,I26+$I9)+J21</f>
+        <f t="shared" ref="J25:O25" ca="1" si="10">MAX(I25+$I8,I26+$I9)+J21</f>
         <v>-5.6913599546576439</v>
       </c>
       <c r="K25">
@@ -962,7 +1120,7 @@
         <v>-15.846390533029677</v>
       </c>
       <c r="P25">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">MAX(O25+$I8,O26+$I9)+P21</f>
         <v>-17.784332512435814</v>
       </c>
     </row>
@@ -1007,6 +1165,82 @@
         <v>-16.973402296219486</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H28" t="str">
+        <f ca="1">IF(H31&gt;H32,$G25,$G26)</f>
+        <v>H</v>
+      </c>
+      <c r="I28" t="str">
+        <f ca="1">IF(I31&gt;I32,$G25,$G26)</f>
+        <v>H</v>
+      </c>
+      <c r="J28" t="str">
+        <f ca="1">IF(J31&gt;J32,$G25,$G26)</f>
+        <v>H</v>
+      </c>
+      <c r="K28" t="str">
+        <f ca="1">IF(K31&gt;K32,$G25,$G26)</f>
+        <v>L</v>
+      </c>
+      <c r="L28" t="str">
+        <f ca="1">IF(L31&gt;L32,$G25,$G26)</f>
+        <v>L</v>
+      </c>
+      <c r="M28" t="str">
+        <f ca="1">IF(M31&gt;M32,$G25,$G26)</f>
+        <v>L</v>
+      </c>
+      <c r="N28" t="str">
+        <f ca="1">IF(N31&gt;N32,$G25,$G26)</f>
+        <v>L</v>
+      </c>
+      <c r="O28" t="str">
+        <f ca="1">IF(O31&gt;O32,$G25,$G26)</f>
+        <v>L</v>
+      </c>
+      <c r="P28" t="str">
+        <f ca="1">MID(L2,IF(P25&gt;P26, 1, 2), 1)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <f ca="1">FIND(H28,$L$2)-1</f>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f ca="1">FIND(I28,$L$2)-1</f>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f ca="1">FIND(J28,$L$2)-1</f>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f ca="1">FIND(K28,$L$2)-1</f>
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <f ca="1">FIND(L28,$L$2)-1</f>
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f ca="1">FIND(M28,$L$2)-1</f>
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f ca="1">FIND(N28,$L$2)-1</f>
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <f ca="1">FIND(O28,$L$2)-1</f>
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <f ca="1">FIND(P28,$L$2)-1</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
@@ -1018,6 +1252,41 @@
       </c>
       <c r="B31">
         <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31">
+        <f ca="1">H25+INDIRECT(ADDRESS(ROW($I8), COLUMN($I8)+I29))</f>
+        <v>-2.5902671654458267</v>
+      </c>
+      <c r="I31">
+        <f ca="1">I25+INDIRECT(ADDRESS(ROW($I8), COLUMN($I8)+J29))</f>
+        <v>-4.487387150331708</v>
+      </c>
+      <c r="J31">
+        <f ca="1">J25+INDIRECT(ADDRESS(ROW($I8), COLUMN($I8)+K29))</f>
+        <v>-6.3845071352175893</v>
+      </c>
+      <c r="K31">
+        <f ca="1">K25+INDIRECT(ADDRESS(ROW($I8), COLUMN($I8)+L29))</f>
+        <v>-8.6870922282116343</v>
+      </c>
+      <c r="L31">
+        <f ca="1">L25+INDIRECT(ADDRESS(ROW($I8), COLUMN($I8)+M29))</f>
+        <v>-10.401890656303561</v>
+      </c>
+      <c r="M31">
+        <f ca="1">M25+INDIRECT(ADDRESS(ROW($I8), COLUMN($I8)+N29))</f>
+        <v>-12.704475749297606</v>
+      </c>
+      <c r="N31">
+        <f ca="1">N25+INDIRECT(ADDRESS(ROW($I8), COLUMN($I8)+O29))</f>
+        <v>-14.236952620595577</v>
+      </c>
+      <c r="O31">
+        <f ca="1">O25+INDIRECT(ADDRESS(ROW($I8), COLUMN($I8)+P29))</f>
+        <v>-16.53953771358962</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
@@ -1029,8 +1298,40 @@
         <f ca="1"/>
         <v>-2.3025850929940455</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <f ca="1">H26+INDIRECT(ADDRESS(ROW($I9), COLUMN($I9)+I29))</f>
+        <v>-3.2188758248682006</v>
+      </c>
+      <c r="I32">
+        <f ca="1">I26+INDIRECT(ADDRESS(ROW($I9), COLUMN($I9)+J29))</f>
+        <v>-5.1159958097540823</v>
+      </c>
+      <c r="J32">
+        <f ca="1">J26+INDIRECT(ADDRESS(ROW($I9), COLUMN($I9)+K29))</f>
+        <v>-6.607650686531799</v>
+      </c>
+      <c r="K32">
+        <f ca="1">K26+INDIRECT(ADDRESS(ROW($I9), COLUMN($I9)+L29))</f>
+        <v>-8.0993055633095157</v>
+      </c>
+      <c r="L32">
+        <f ca="1">L26+INDIRECT(ADDRESS(ROW($I9), COLUMN($I9)+M29))</f>
+        <v>-10.219569099509606</v>
+      </c>
+      <c r="M32">
+        <f ca="1">M26+INDIRECT(ADDRESS(ROW($I9), COLUMN($I9)+N29))</f>
+        <v>-11.934367527601532</v>
+      </c>
+      <c r="N32">
+        <f ca="1">N26+INDIRECT(ADDRESS(ROW($I9), COLUMN($I9)+O29))</f>
+        <v>-14.054631063801622</v>
+      </c>
+      <c r="O32">
+        <f ca="1">O26+INDIRECT(ADDRESS(ROW($I9), COLUMN($I9)+P29))</f>
+        <v>-15.769429491893549</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <f ca="1"/>
         <v>-3.7942399697717626</v>
@@ -1040,7 +1341,7 @@
         <v>-4.1997050778799272</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <f ca="1"/>
         <v>-5.6913599546576439</v>
@@ -1050,7 +1351,7 @@
         <v>-6.0968250627658085</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <f ca="1"/>
         <v>-7.9939450476516898</v>
@@ -1060,7 +1361,7 @@
         <v>-7.5884799395435252</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <f ca="1"/>
         <v>-9.7087434757436153</v>
@@ -1070,7 +1371,7 @@
         <v>-9.7087434757436153</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <f ca="1"/>
         <v>-12.01132856873766</v>
@@ -1080,7 +1381,7 @@
         <v>-11.423541903835542</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <f ca="1"/>
         <v>-13.543805440035632</v>
@@ -1090,7 +1391,7 @@
         <v>-13.543805440035632</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <f ca="1"/>
         <v>-15.846390533029677</v>
@@ -1100,7 +1401,7 @@
         <v>-15.258603868127558</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <f ca="1"/>
         <v>-17.784332512435814</v>
@@ -1110,7 +1411,955 @@
         <v>-16.973402296219486</v>
       </c>
     </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f ca="1">H29</f>
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <f t="shared" ref="B44:I44" ca="1" si="12">I29</f>
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ca="1" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ca="1" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <f t="shared" ca="1" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ca="1" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <f t="shared" ca="1" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <f t="shared" ca="1" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.8</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.2</v>
+      </c>
+      <c r="B4">
+        <v>0.7</v>
+      </c>
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.1</v>
+      </c>
+      <c r="B5">
+        <v>0.3</v>
+      </c>
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5">
+        <f>LN(A15)</f>
+        <v>-0.51082562376599072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6">
+        <f>LN(B15)</f>
+        <v>-1.6094379124341003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <f>LN(C15)</f>
+        <v>-1.6094379124341003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0.3</v>
+      </c>
+      <c r="L9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.1</v>
+      </c>
+      <c r="B10">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="C11">
+        <v>0.8</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11">
+        <f>LN(A3)</f>
+        <v>-0.22314355131420971</v>
+      </c>
+      <c r="N11">
+        <f>LN(B3)</f>
+        <v>-2.3025850929940455</v>
+      </c>
+      <c r="O11">
+        <f>LN(C3)</f>
+        <v>-2.3025850929940455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M12:O12" si="0">LN(A4)</f>
+        <v>-1.6094379124341003</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>-2.3025850929940455</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M13:O13" si="1">LN(A5)</f>
+        <v>-2.3025850929940455</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>-1.2039728043259361</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>-0.51082562376599072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.6</v>
+      </c>
+      <c r="B15">
+        <v>0.2</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
+      </c>
+      <c r="L15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17">
+        <f>LN(A9)</f>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="N17">
+        <v>-128</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ref="O17" si="2">LN(C9)</f>
+        <v>-1.2039728043259361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="L18" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18" si="3">LN(A10)</f>
+        <v>-2.3025850929940455</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ref="N18:N19" si="4">LN(B10)</f>
+        <v>-0.10536051565782628</v>
+      </c>
+      <c r="O18">
+        <v>-128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f>L23</f>
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ref="B19:F19" si="5">M23</f>
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19">
+        <v>-128</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="4"/>
+        <v>-1.6094379124341003</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ref="O19" si="6">LN(C11)</f>
+        <v>-0.22314355131420971</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N22" t="s">
+        <v>31</v>
+      </c>
+      <c r="O22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P22" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23">
+        <f>(FIND(L22,$M2)-1)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ref="M23:Q23" si="7">(FIND(M22,$M2)-1)/2</f>
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24">
+        <f ca="1">INDIRECT(ADDRESS(ROW($M17), COLUMN($M$17)+L$23))</f>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:Q24" ca="1" si="8">INDIRECT(ADDRESS(ROW($M17), COLUMN($M$17)+M$23))</f>
+        <v>-1.2039728043259361</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.35667494393873245</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ca="1" si="8"/>
+        <v>-1.2039728043259361</v>
+      </c>
+      <c r="P24">
+        <f t="shared" ca="1" si="8"/>
+        <v>-1.2039728043259361</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" ca="1" si="8"/>
+        <v>-128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K25" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ref="L25:Q26" ca="1" si="9">INDIRECT(ADDRESS(ROW($M18), COLUMN($M$17)+L$23))</f>
+        <v>-2.3025850929940455</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ca="1" si="9"/>
+        <v>-128</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ca="1" si="9"/>
+        <v>-2.3025850929940455</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ca="1" si="9"/>
+        <v>-128</v>
+      </c>
+      <c r="P25">
+        <f t="shared" ca="1" si="9"/>
+        <v>-128</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.10536051565782628</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K26" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ca="1" si="9"/>
+        <v>-128</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.22314355131420971</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ca="1" si="9"/>
+        <v>-128</v>
+      </c>
+      <c r="O26">
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.22314355131420971</v>
+      </c>
+      <c r="P26">
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.22314355131420971</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ca="1" si="9"/>
+        <v>-1.6094379124341003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28">
+        <f ca="1">L24+M5</f>
+        <v>-0.86750056770472317</v>
+      </c>
+      <c r="M28">
+        <f ca="1">MAX(L28+$M11+M24,L29+$M12+M24,L30+$M13+M24)</f>
+        <v>-2.294616923344869</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ref="N28:Q28" ca="1" si="10">MAX(M28+$M11+N24,M29+$M12+N24,M30+$M13+N24)</f>
+        <v>-2.8744354185978112</v>
+      </c>
+      <c r="O28">
+        <f t="shared" ca="1" si="10"/>
+        <v>-4.3015517742379572</v>
+      </c>
+      <c r="P28">
+        <f t="shared" ca="1" si="10"/>
+        <v>-5.7286681298781028</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" ca="1" si="10"/>
+        <v>-133.95181168119231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="K29" t="s">
+        <v>29</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ref="L29:L30" ca="1" si="11">L25+M6</f>
+        <v>-3.9120230054281455</v>
+      </c>
+      <c r="M29">
+        <f ca="1">MAX(L28+$N11+M25,L29+$N12+M25,L30+$N13+M25)</f>
+        <v>-131.17008566069876</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N29:Q29" ca="1" si="12">MAX(M28+$N11+N25,M29+$N12+N25,M30+$N13+N25)</f>
+        <v>-6.8997871093329604</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ca="1" si="12"/>
+        <v>-133.17702051159185</v>
+      </c>
+      <c r="P29">
+        <f t="shared" ca="1" si="12"/>
+        <v>-134.604136867232</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" ca="1" si="12"/>
+        <v>-7.4434665579700283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f ca="1">L37</f>
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ref="B30:F30" ca="1" si="13">M37</f>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ca="1" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ca="1" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ca="1" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L30">
+        <f t="shared" ca="1" si="11"/>
+        <v>-129.60943791243409</v>
+      </c>
+      <c r="M30">
+        <f ca="1">MAX(L28+$O11+M26,L29+$O12+M26,L30+$O13+M26)</f>
+        <v>-3.3932292120129786</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ref="N30:Q30" ca="1" si="14">MAX(M28+$O11+N26,M29+$O12+N26,M30+$O13+N26)</f>
+        <v>-131.90405483577896</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ca="1" si="14"/>
+        <v>-5.4001640629060663</v>
+      </c>
+      <c r="P30">
+        <f t="shared" ca="1" si="14"/>
+        <v>-6.1341332379862665</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" ca="1" si="14"/>
+        <v>-8.2543967741863575</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L32">
+        <f ca="1">EXP(L28)</f>
+        <v>0.41999999999999993</v>
+      </c>
+      <c r="M32">
+        <f ca="1">EXP(M28)</f>
+        <v>0.10079999999999999</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ref="N32:Q32" ca="1" si="15">EXP(N28)</f>
+        <v>5.6447999999999991E-2</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ca="1" si="15"/>
+        <v>1.3547519999999993E-2</v>
+      </c>
+      <c r="P32">
+        <f t="shared" ca="1" si="15"/>
+        <v>3.2514047999999988E-3</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" ca="1" si="15"/>
+        <v>6.6906351206516385E-59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ref="L33:M34" ca="1" si="16">EXP(L29)</f>
+        <v>2.0000000000000011E-2</v>
+      </c>
+      <c r="M33">
+        <f t="shared" ca="1" si="16"/>
+        <v>1.0803279365098237E-57</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ref="N33:Q33" ca="1" si="17">EXP(N29)</f>
+        <v>1.0079999999999998E-3</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ca="1" si="17"/>
+        <v>1.4519607466692019E-58</v>
+      </c>
+      <c r="P33">
+        <f t="shared" ca="1" si="17"/>
+        <v>3.4847057920060636E-59</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" ca="1" si="17"/>
+        <v>5.8525286400000042E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f ca="1">L28</f>
+        <v>-0.86750056770472317</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ref="B34:F34" ca="1" si="18">M28</f>
+        <v>-2.294616923344869</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ca="1" si="18"/>
+        <v>-2.8744354185978112</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ca="1" si="18"/>
+        <v>-4.3015517742379572</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ca="1" si="18"/>
+        <v>-5.7286681298781028</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ca="1" si="18"/>
+        <v>-133.95181168119231</v>
+      </c>
+      <c r="L34">
+        <f t="shared" ca="1" si="16"/>
+        <v>5.1444187452848885E-57</v>
+      </c>
+      <c r="M34">
+        <f t="shared" ca="1" si="16"/>
+        <v>3.3599999999999998E-2</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ref="N34:Q34" ca="1" si="19">EXP(N30)</f>
+        <v>5.1855740952471321E-58</v>
+      </c>
+      <c r="O34">
+        <f t="shared" ca="1" si="19"/>
+        <v>4.5158400000000001E-3</v>
+      </c>
+      <c r="P34">
+        <f t="shared" ca="1" si="19"/>
+        <v>2.1676032000000007E-3</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" ca="1" si="19"/>
+        <v>2.601123840000001E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" ref="A35:A36" ca="1" si="20">L29</f>
+        <v>-3.9120230054281455</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ref="B35:B36" ca="1" si="21">M29</f>
+        <v>-131.17008566069876</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:C36" ca="1" si="22">N29</f>
+        <v>-6.8997871093329604</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:D36" ca="1" si="23">O29</f>
+        <v>-133.17702051159185</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ref="E35:E36" ca="1" si="24">P29</f>
+        <v>-134.604136867232</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ref="F35:F36" ca="1" si="25">Q29</f>
+        <v>-7.4434665579700283</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" ca="1" si="20"/>
+        <v>-129.60943791243409</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ca="1" si="21"/>
+        <v>-3.3932292120129786</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ca="1" si="22"/>
+        <v>-131.90405483577896</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ca="1" si="23"/>
+        <v>-5.4001640629060663</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ca="1" si="24"/>
+        <v>-6.1341332379862665</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ca="1" si="25"/>
+        <v>-8.2543967741863575</v>
+      </c>
+      <c r="J36" t="s">
+        <v>40</v>
+      </c>
+      <c r="L36" t="str">
+        <f ca="1">IF(MAX(L39:L41)=L39, $K28, IF(MAX(L39:L41)=L40, $K29, $K30))</f>
+        <v>A1</v>
+      </c>
+      <c r="M36" t="str">
+        <f ca="1">IF(MAX(M39:M41)=M39, $K28, IF(MAX(M39:M41)=M40, $K29, $K30))</f>
+        <v>A1</v>
+      </c>
+      <c r="N36" t="str">
+        <f ca="1">IF(MAX(N39:N41)=N39, $K28, IF(MAX(N39:N41)=N40, $K29, $K30))</f>
+        <v>A1</v>
+      </c>
+      <c r="O36" t="str">
+        <f ca="1">IF(MAX(O39:O41)=O39, $K28, IF(MAX(O39:O41)=O40, $K29, $K30))</f>
+        <v>A3</v>
+      </c>
+      <c r="P36" t="str">
+        <f ca="1">IF(MAX(P39:P41)=P39, $K28, IF(MAX(P39:P41)=P40, $K29, $K30))</f>
+        <v>A3</v>
+      </c>
+      <c r="Q36" t="str">
+        <f ca="1">IF(MAX(Q28:Q30)=Q28, K28, IF(MAX(Q28:Q30)=Q29, K29, K30))</f>
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L37">
+        <f t="shared" ref="L37:Q37" ca="1" si="26">(FIND(L36,$M$1)-1)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f t="shared" ca="1" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ca="1" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f t="shared" ca="1" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P37">
+        <f t="shared" ca="1" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" ca="1" si="26"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>39</v>
+      </c>
+      <c r="L39">
+        <f ca="1">L28+INDIRECT(ADDRESS(ROW($M11), COLUMN($M11)+M37))</f>
+        <v>-1.0906441190189329</v>
+      </c>
+      <c r="M39">
+        <f ca="1">M28+INDIRECT(ADDRESS(ROW($M11), COLUMN($M11)+N37))</f>
+        <v>-2.5177604746590787</v>
+      </c>
+      <c r="N39">
+        <f ca="1">N28+INDIRECT(ADDRESS(ROW($M11), COLUMN($M11)+O37))</f>
+        <v>-5.1770205115918566</v>
+      </c>
+      <c r="O39">
+        <f ca="1">O28+INDIRECT(ADDRESS(ROW($M11), COLUMN($M11)+P37))</f>
+        <v>-6.6041368672320022</v>
+      </c>
+      <c r="P39">
+        <f ca="1">P28+INDIRECT(ADDRESS(ROW($M11), COLUMN($M11)+Q37))</f>
+        <v>-8.0312532228721487</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L40">
+        <f ca="1">L29+INDIRECT(ADDRESS(ROW($M12), COLUMN($M12)+M37))</f>
+        <v>-5.521460917862246</v>
+      </c>
+      <c r="M40">
+        <f ca="1">M29+INDIRECT(ADDRESS(ROW($M12), COLUMN($M12)+N37))</f>
+        <v>-132.77952357313285</v>
+      </c>
+      <c r="N40">
+        <f ca="1">N29+INDIRECT(ADDRESS(ROW($M12), COLUMN($M12)+O37))</f>
+        <v>-9.2023722023270054</v>
+      </c>
+      <c r="O40">
+        <f ca="1">O29+INDIRECT(ADDRESS(ROW($M12), COLUMN($M12)+P37))</f>
+        <v>-135.47960560458588</v>
+      </c>
+      <c r="P40">
+        <f ca="1">P29+INDIRECT(ADDRESS(ROW($M12), COLUMN($M12)+Q37))</f>
+        <v>-134.96081181117074</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <f ca="1">L30+INDIRECT(ADDRESS(ROW($M13), COLUMN($M13)+M37))</f>
+        <v>-131.91202300542813</v>
+      </c>
+      <c r="M41">
+        <f ca="1">M30+INDIRECT(ADDRESS(ROW($M13), COLUMN($M13)+N37))</f>
+        <v>-5.6958143050070245</v>
+      </c>
+      <c r="N41">
+        <f ca="1">N30+INDIRECT(ADDRESS(ROW($M13), COLUMN($M13)+O37))</f>
+        <v>-132.41488045954495</v>
+      </c>
+      <c r="O41">
+        <f ca="1">O30+INDIRECT(ADDRESS(ROW($M13), COLUMN($M13)+P37))</f>
+        <v>-5.9109896866720568</v>
+      </c>
+      <c r="P41">
+        <f ca="1">P30+INDIRECT(ADDRESS(ROW($M13), COLUMN($M13)+Q37))</f>
+        <v>-7.3381060423122024</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>